<commit_message>
Reverted modularization until further notice
</commit_message>
<xml_diff>
--- a/print_docs/excel/excel_template/KEMSA Customer Order Form.xlsx
+++ b/print_docs/excel/excel_template/KEMSA Customer Order Form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\HCMP-1\print_docs\excel\excel_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Karsan\Work\HCMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2893,9 +2893,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="172" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    <numFmt numFmtId="173" formatCode="0.00;[Red]0.00"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    <numFmt numFmtId="166" formatCode="0.00;[Red]0.00"/>
   </numFmts>
   <fonts count="46" x14ac:knownFonts="1">
     <font>
@@ -3775,7 +3775,7 @@
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3790,7 +3790,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3806,7 +3806,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="18" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3832,7 +3832,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3848,7 +3848,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3862,13 +3862,13 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="171" fontId="24" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="24" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="24" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3879,7 +3879,7 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="171" fontId="10" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3905,13 +3905,13 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="8" fillId="6" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="8" fillId="6" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3945,7 +3945,7 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3963,7 +3963,7 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4033,7 +4033,7 @@
     <xf numFmtId="0" fontId="28" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="8" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="8" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -4043,7 +4043,7 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4153,7 +4153,7 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -4203,7 +4203,7 @@
     <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -4361,7 +4361,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="171" fontId="39" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -4371,7 +4371,7 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4445,13 +4445,13 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="14" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="14" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="14" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4505,10 +4505,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="14" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -4539,8 +4539,56 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="14" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -4597,54 +4645,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="14" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6195,8 +6195,8 @@
   </sheetPr>
   <dimension ref="A1:L806"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6246,7 +6246,7 @@
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="29"/>
-      <c r="C4" s="305"/>
+      <c r="C4" s="321"/>
       <c r="D4" s="37"/>
       <c r="E4" s="238" t="s">
         <v>343</v>
@@ -6255,14 +6255,14 @@
       <c r="G4" s="38" t="s">
         <v>333</v>
       </c>
-      <c r="H4" s="306"/>
-      <c r="I4" s="307"/>
-      <c r="J4" s="308"/>
+      <c r="H4" s="322"/>
+      <c r="I4" s="323"/>
+      <c r="J4" s="324"/>
       <c r="K4" s="36"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="29"/>
-      <c r="C5" s="305"/>
+      <c r="C5" s="321"/>
       <c r="D5" s="37"/>
       <c r="E5" s="239" t="s">
         <v>344</v>
@@ -6271,14 +6271,14 @@
       <c r="G5" s="39" t="s">
         <v>334</v>
       </c>
-      <c r="H5" s="309"/>
-      <c r="I5" s="310"/>
-      <c r="J5" s="311"/>
+      <c r="H5" s="325"/>
+      <c r="I5" s="326"/>
+      <c r="J5" s="327"/>
       <c r="K5" s="36"/>
     </row>
     <row r="6" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B6" s="29"/>
-      <c r="C6" s="305"/>
+      <c r="C6" s="321"/>
       <c r="D6" s="37"/>
       <c r="E6" s="239" t="s">
         <v>345</v>
@@ -6287,14 +6287,14 @@
       <c r="G6" s="39" t="s">
         <v>335</v>
       </c>
-      <c r="H6" s="309"/>
-      <c r="I6" s="310"/>
-      <c r="J6" s="311"/>
+      <c r="H6" s="325"/>
+      <c r="I6" s="326"/>
+      <c r="J6" s="327"/>
       <c r="K6" s="36"/>
     </row>
     <row r="7" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="29"/>
-      <c r="C7" s="305"/>
+      <c r="C7" s="321"/>
       <c r="D7" s="37"/>
       <c r="E7" s="239" t="s">
         <v>346</v>
@@ -6303,14 +6303,14 @@
       <c r="G7" s="39" t="s">
         <v>336</v>
       </c>
-      <c r="H7" s="309"/>
-      <c r="I7" s="310"/>
-      <c r="J7" s="311"/>
+      <c r="H7" s="325"/>
+      <c r="I7" s="326"/>
+      <c r="J7" s="327"/>
       <c r="K7" s="36"/>
     </row>
     <row r="8" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="29"/>
-      <c r="C8" s="305"/>
+      <c r="C8" s="321"/>
       <c r="D8" s="31"/>
       <c r="E8" s="240" t="s">
         <v>347</v>
@@ -6319,9 +6319,9 @@
       <c r="G8" s="40" t="s">
         <v>342</v>
       </c>
-      <c r="H8" s="302"/>
-      <c r="I8" s="303"/>
-      <c r="J8" s="304"/>
+      <c r="H8" s="318"/>
+      <c r="I8" s="319"/>
+      <c r="J8" s="320"/>
       <c r="K8" s="36"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
@@ -6351,13 +6351,13 @@
     <row r="11" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="29"/>
       <c r="C11" s="249"/>
-      <c r="D11" s="321" t="s">
+      <c r="D11" s="305" t="s">
         <v>341</v>
       </c>
-      <c r="E11" s="320"/>
-      <c r="F11" s="320"/>
-      <c r="G11" s="320"/>
-      <c r="H11" s="322"/>
+      <c r="E11" s="304"/>
+      <c r="F11" s="304"/>
+      <c r="G11" s="304"/>
+      <c r="H11" s="306"/>
       <c r="I11" s="41"/>
       <c r="J11" s="35"/>
       <c r="K11" s="36"/>
@@ -6365,11 +6365,11 @@
     <row r="12" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="29"/>
       <c r="C12" s="249"/>
-      <c r="D12" s="323"/>
-      <c r="E12" s="324"/>
-      <c r="F12" s="324"/>
-      <c r="G12" s="324"/>
-      <c r="H12" s="325"/>
+      <c r="D12" s="307"/>
+      <c r="E12" s="308"/>
+      <c r="F12" s="308"/>
+      <c r="G12" s="308"/>
+      <c r="H12" s="309"/>
       <c r="I12" s="41"/>
       <c r="J12" s="35"/>
       <c r="K12" s="36"/>
@@ -6377,13 +6377,13 @@
     <row r="13" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="29"/>
       <c r="C13" s="249"/>
-      <c r="D13" s="320" t="s">
+      <c r="D13" s="304" t="s">
         <v>833</v>
       </c>
-      <c r="E13" s="320"/>
-      <c r="F13" s="320"/>
-      <c r="G13" s="320"/>
-      <c r="H13" s="320"/>
+      <c r="E13" s="304"/>
+      <c r="F13" s="304"/>
+      <c r="G13" s="304"/>
+      <c r="H13" s="304"/>
       <c r="I13" s="41"/>
       <c r="J13" s="35"/>
       <c r="K13" s="36"/>
@@ -6404,16 +6404,16 @@
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="29"/>
-      <c r="C15" s="326" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="327"/>
-      <c r="E15" s="327"/>
-      <c r="F15" s="327"/>
-      <c r="G15" s="327"/>
-      <c r="H15" s="327"/>
-      <c r="I15" s="327"/>
-      <c r="J15" s="328"/>
+      <c r="C15" s="310" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="311"/>
+      <c r="E15" s="311"/>
+      <c r="F15" s="311"/>
+      <c r="G15" s="311"/>
+      <c r="H15" s="311"/>
+      <c r="I15" s="311"/>
+      <c r="J15" s="312"/>
       <c r="K15" s="36"/>
     </row>
     <row r="16" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -6463,11 +6463,13 @@
       <c r="G17" s="55">
         <v>265</v>
       </c>
-      <c r="H17" s="16"/>
+      <c r="H17" s="16">
+        <v>10</v>
+      </c>
       <c r="I17" s="56"/>
       <c r="J17" s="57">
         <f t="shared" ref="J17:J92" si="0">G17*H17</f>
-        <v>0</v>
+        <v>2650</v>
       </c>
       <c r="K17" s="36"/>
     </row>
@@ -11238,16 +11240,16 @@
       <c r="B190" s="99"/>
       <c r="C190" s="100"/>
       <c r="D190" s="101"/>
-      <c r="E190" s="329" t="s">
+      <c r="E190" s="313" t="s">
         <v>828</v>
       </c>
-      <c r="F190" s="330"/>
-      <c r="G190" s="330"/>
-      <c r="H190" s="330"/>
+      <c r="F190" s="314"/>
+      <c r="G190" s="314"/>
+      <c r="H190" s="314"/>
       <c r="I190" s="102"/>
       <c r="J190" s="103">
         <f>SUM(J17:J189)</f>
-        <v>0</v>
+        <v>2650</v>
       </c>
       <c r="K190" s="36"/>
     </row>
@@ -11265,10 +11267,10 @@
     </row>
     <row r="192" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" s="111"/>
-      <c r="C192" s="314" t="s">
+      <c r="C192" s="330" t="s">
         <v>504</v>
       </c>
-      <c r="D192" s="315"/>
+      <c r="D192" s="331"/>
       <c r="E192" s="112"/>
       <c r="F192" s="112"/>
       <c r="G192" s="112"/>
@@ -15984,12 +15986,12 @@
       <c r="B367" s="99"/>
       <c r="C367" s="158"/>
       <c r="D367" s="159"/>
-      <c r="E367" s="312" t="s">
+      <c r="E367" s="328" t="s">
         <v>829</v>
       </c>
-      <c r="F367" s="312"/>
-      <c r="G367" s="312"/>
-      <c r="H367" s="313"/>
+      <c r="F367" s="328"/>
+      <c r="G367" s="328"/>
+      <c r="H367" s="329"/>
       <c r="I367" s="102"/>
       <c r="J367" s="160">
         <f>SUM(J193:J366)</f>
@@ -16011,10 +16013,10 @@
     </row>
     <row r="369" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B369" s="50"/>
-      <c r="C369" s="316" t="s">
+      <c r="C369" s="300" t="s">
         <v>698</v>
       </c>
-      <c r="D369" s="317"/>
+      <c r="D369" s="301"/>
       <c r="E369" s="167"/>
       <c r="F369" s="167"/>
       <c r="G369" s="167"/>
@@ -16567,12 +16569,12 @@
       <c r="B390" s="50"/>
       <c r="C390" s="158"/>
       <c r="D390" s="179"/>
-      <c r="E390" s="331" t="s">
+      <c r="E390" s="315" t="s">
         <v>830</v>
       </c>
-      <c r="F390" s="331"/>
-      <c r="G390" s="331"/>
-      <c r="H390" s="331"/>
+      <c r="F390" s="315"/>
+      <c r="G390" s="315"/>
+      <c r="H390" s="315"/>
       <c r="I390" s="102"/>
       <c r="J390" s="180">
         <f>SUM(J370:J389)</f>
@@ -16594,10 +16596,10 @@
     </row>
     <row r="392" spans="2:11" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B392" s="185"/>
-      <c r="C392" s="318" t="s">
+      <c r="C392" s="302" t="s">
         <v>666</v>
       </c>
-      <c r="D392" s="319"/>
+      <c r="D392" s="303"/>
       <c r="E392" s="186"/>
       <c r="F392" s="186"/>
       <c r="G392" s="186"/>
@@ -16988,12 +16990,12 @@
       <c r="B407" s="29"/>
       <c r="C407" s="252"/>
       <c r="D407" s="195"/>
-      <c r="E407" s="300" t="s">
+      <c r="E407" s="316" t="s">
         <v>699</v>
       </c>
-      <c r="F407" s="300"/>
-      <c r="G407" s="300"/>
-      <c r="H407" s="300"/>
+      <c r="F407" s="316"/>
+      <c r="G407" s="316"/>
+      <c r="H407" s="316"/>
       <c r="I407" s="196"/>
       <c r="J407" s="197">
         <f>SUM(J393:J406)</f>
@@ -17018,15 +17020,15 @@
       <c r="C409" s="252"/>
       <c r="D409" s="195"/>
       <c r="E409" s="195"/>
-      <c r="F409" s="301" t="s">
+      <c r="F409" s="317" t="s">
         <v>697</v>
       </c>
-      <c r="G409" s="301"/>
-      <c r="H409" s="301"/>
+      <c r="G409" s="317"/>
+      <c r="H409" s="317"/>
       <c r="I409" s="200"/>
       <c r="J409" s="201">
         <f>J190+J367+J390+J407</f>
-        <v>0</v>
+        <v>2650</v>
       </c>
       <c r="K409" s="36"/>
     </row>
@@ -20095,13 +20097,6 @@
   </sheetData>
   <sheetProtection password="9F39" sheet="1" autoFilter="0"/>
   <mergeCells count="17">
-    <mergeCell ref="C369:D369"/>
-    <mergeCell ref="C392:D392"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="D11:H12"/>
-    <mergeCell ref="C15:J15"/>
-    <mergeCell ref="E190:H190"/>
-    <mergeCell ref="E390:H390"/>
     <mergeCell ref="E407:H407"/>
     <mergeCell ref="F409:H409"/>
     <mergeCell ref="H8:J8"/>
@@ -20112,6 +20107,13 @@
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="E367:H367"/>
     <mergeCell ref="C192:D192"/>
+    <mergeCell ref="C369:D369"/>
+    <mergeCell ref="C392:D392"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="D11:H12"/>
+    <mergeCell ref="C15:J15"/>
+    <mergeCell ref="E190:H190"/>
+    <mergeCell ref="E390:H390"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E8" r:id="rId1"/>

</xml_diff>